<commit_message>
Included last two seed measurements for species that needed to be weighed (OENFIL & RUBSPP).
</commit_message>
<xml_diff>
--- a/SR_SB_VEG_Traits_Dataset.xlsx
+++ b/SR_SB_VEG_Traits_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wynnekat/SR---New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D718BD-A5CF-F646-8B86-6B579A051FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A06552C-B998-4D43-B878-1B32C60A134D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="740" windowWidth="28480" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10980" yWindow="740" windowWidth="18420" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2930,9 +2930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10085,6 +10085,9 @@
       <c r="N135" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="O135" s="20">
+        <v>8.9469000000000007E-3</v>
+      </c>
       <c r="R135" s="5"/>
       <c r="Z135" s="7" t="s">
         <v>34</v>
@@ -11445,7 +11448,9 @@
       <c r="N163" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O163" s="5"/>
+      <c r="O163" s="5">
+        <v>2.7023799999999999E-3</v>
+      </c>
       <c r="P163" s="5"/>
       <c r="Q163" s="5"/>
       <c r="R163" s="5"/>

</xml_diff>